<commit_message>
Solving the instrument update bug on backend added normalisation for various conditions
</commit_message>
<xml_diff>
--- a/services/api/templates/master_report_template.xlsx
+++ b/services/api/templates/master_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE0F78E-912D-8243-B464-5DE5DE3F70F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C466D702-B6A1-2A42-80C9-B8C138AD532B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{4990D55F-8C01-414D-8D14-99C9A7F325C1}"/>
   </bookViews>
@@ -198,6 +198,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -219,7 +220,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,58 +632,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="e" vm="1">
+      <c r="A1" s="6" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
@@ -695,8 +695,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
@@ -786,16 +786,16 @@
       <c r="G14" s="1"/>
     </row>
     <row r="21" spans="9:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="I21" s="11"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="23" spans="9:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="I23" s="11"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="25" spans="9:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="I25" s="11"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="27" spans="9:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="I27" s="11"/>
+      <c r="I27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>